<commit_message>
Ajout de la gestion admin sur les boutons de modification/suppression des congés
</commit_message>
<xml_diff>
--- a/PlanningLabo/Consignes de paie VIERGE.xlsx
+++ b/PlanningLabo/Consignes de paie VIERGE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B08324-B12B-47D6-BD56-9BB4DFDE6FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4672362-3258-419E-96D0-D67D0C4E7F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{DC145B23-0354-4A64-B1E4-DC69857A4EB3}"/>
   </bookViews>
@@ -224,7 +224,7 @@
     <numFmt numFmtId="167" formatCode="00.00"/>
     <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;€&quot;;[Red]#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,12 +272,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Aptos Display"/>
@@ -287,11 +281,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Aptos Display"/>
       <family val="2"/>
     </font>
@@ -306,13 +295,6 @@
       <b/>
       <i/>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color rgb="FF0070C0"/>
       <name val="Aptos Display"/>
       <family val="2"/>
@@ -346,18 +328,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -469,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -507,45 +485,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -563,94 +526,72 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -662,13 +603,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -677,28 +618,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -707,16 +648,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1053,16 +994,16 @@
   </sheetPr>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="48" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="40" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="48" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="40" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" customWidth="1"/>
@@ -1075,62 +1016,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="42" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90" t="s">
+      <c r="F1" s="77"/>
+      <c r="G1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="90" t="s">
+      <c r="H1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
       <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="91" t="s">
+      <c r="N1" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="90" t="s">
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="90"/>
+      <c r="R1" s="77"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
       <c r="I2" s="4">
         <v>0.1</v>
       </c>
@@ -1155,8 +1096,8 @@
       <c r="P2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -1179,16 +1120,16 @@
       <c r="H3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="82"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="69"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -1203,20 +1144,20 @@
       <c r="D4" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="84"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="71"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
@@ -1225,28 +1166,28 @@
       <c r="B5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="10">
         <v>86.67</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="80" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="R5" s="80"/>
+      <c r="R5" s="67"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
@@ -1261,24 +1202,24 @@
       <c r="D6" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="46" t="s">
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="R6" s="47">
+      <c r="R6" s="39">
         <v>76.3</v>
       </c>
     </row>
@@ -1289,28 +1230,28 @@
       <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="85"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="72"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -1319,28 +1260,28 @@
       <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="61"/>
-      <c r="Q8" s="85"/>
-      <c r="R8" s="85"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="72"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
@@ -1355,26 +1296,26 @@
       <c r="D9" s="10">
         <v>123.2</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="80" t="s">
+      <c r="I9" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="80" t="s">
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="67"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="R9" s="80"/>
+      <c r="R9" s="67"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
@@ -1383,26 +1324,26 @@
       <c r="B10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="10">
         <v>121.33</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
@@ -1411,28 +1352,28 @@
       <c r="B11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="85"/>
-      <c r="R11" s="85"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="72"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
@@ -1441,28 +1382,28 @@
       <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="79"/>
-      <c r="R12" s="79"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -1477,20 +1418,20 @@
       <c r="D13" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="87"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="74"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
@@ -1499,26 +1440,26 @@
       <c r="B14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="10">
         <v>60</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="72"/>
+      <c r="R14" s="72"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
@@ -1527,24 +1468,24 @@
       <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="77"/>
-      <c r="R15" s="78"/>
+      <c r="C15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="64"/>
+      <c r="R15" s="65"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
@@ -1553,28 +1494,28 @@
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="10">
         <v>30</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="46" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="R16" s="47">
+      <c r="R16" s="39">
         <v>77.3</v>
       </c>
     </row>
@@ -1585,30 +1526,30 @@
       <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="22">
         <v>45232</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="68"/>
-      <c r="R17" s="69"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="56"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
@@ -1617,32 +1558,32 @@
       <c r="B18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="18" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="10">
         <v>121.33</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="22">
         <v>44805</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="22">
         <v>45535</v>
       </c>
-      <c r="G18" s="16"/>
+      <c r="G18" s="14"/>
       <c r="H18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="68"/>
-      <c r="R18" s="69"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="56"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
@@ -1651,28 +1592,28 @@
       <c r="B19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="10">
         <v>80</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="46" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="R19" s="47">
+      <c r="R19" s="39">
         <v>77.3</v>
       </c>
     </row>
@@ -1683,32 +1624,32 @@
       <c r="B20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="18" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="22">
         <v>45170</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="22">
         <v>45900</v>
       </c>
-      <c r="G20" s="16"/>
+      <c r="G20" s="14"/>
       <c r="H20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="70"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
@@ -1717,32 +1658,32 @@
       <c r="B21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="23" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="21">
         <v>45170</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="21">
         <v>45900</v>
       </c>
-      <c r="G21" s="16"/>
+      <c r="G21" s="14"/>
       <c r="H21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="65"/>
-      <c r="R21" s="65"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="52"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -1751,32 +1692,32 @@
       <c r="B22" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="23" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="21">
         <v>45170</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="21">
         <v>45900</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="14"/>
       <c r="H22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="67"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="53"/>
+      <c r="R22" s="54"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
@@ -1785,64 +1726,64 @@
       <c r="B23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="18" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="22">
         <v>45170</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="22">
         <v>45900</v>
       </c>
-      <c r="G23" s="16"/>
+      <c r="G23" s="14"/>
       <c r="H23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="66"/>
-      <c r="R23" s="67"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="54"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
+      <c r="A24" s="24">
         <v>256</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="31">
-        <v>151.66999999999999</v>
-      </c>
-      <c r="E24" s="27">
+      <c r="C24" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="26">
+        <v>151.66999999999999</v>
+      </c>
+      <c r="E24" s="22">
         <v>45183</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="32" t="s">
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="66"/>
-      <c r="R24" s="67"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="54"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
@@ -1854,23 +1795,23 @@
       <c r="C25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="34">
-        <v>151.66999999999999</v>
-      </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="73"/>
-      <c r="R25" s="74"/>
+      <c r="D25" s="29">
+        <v>151.66999999999999</v>
+      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="61"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
@@ -1885,20 +1826,20 @@
       <c r="D26" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="61"/>
-      <c r="Q26" s="73"/>
-      <c r="R26" s="74"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="61"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
@@ -1910,26 +1851,26 @@
       <c r="C27" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="29">
         <v>12</v>
       </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="73"/>
-      <c r="R27" s="74"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="61"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="40">
+      <c r="A28" s="33">
         <v>268</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -1941,93 +1882,93 @@
       <c r="D28" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="44" t="s">
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="64"/>
-      <c r="Q28" s="73"/>
-      <c r="R28" s="74"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="61"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="40">
+      <c r="A29" s="33">
         <v>270</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="23" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="21">
         <v>45516</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="21">
         <v>45880</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="44" t="s">
+      <c r="G29" s="31"/>
+      <c r="H29" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="64"/>
-      <c r="Q29" s="73"/>
-      <c r="R29" s="74"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="61"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="40">
+      <c r="A30" s="33">
         <v>271</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="23" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E30" s="26">
+      <c r="E30" s="21">
         <v>45516</v>
       </c>
-      <c r="F30" s="26">
+      <c r="F30" s="21">
         <v>45880</v>
       </c>
-      <c r="G30" s="36"/>
-      <c r="H30" s="44" t="s">
+      <c r="G30" s="31"/>
+      <c r="H30" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="64"/>
-      <c r="Q30" s="73"/>
-      <c r="R30" s="74"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="61"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="40">
+      <c r="A31" s="33">
         <v>272</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -2039,91 +1980,91 @@
       <c r="D31" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E31" s="41">
+      <c r="E31" s="34">
         <v>45539</v>
       </c>
-      <c r="F31" s="42"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="38"/>
-      <c r="N31" s="59"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="64"/>
-      <c r="Q31" s="75"/>
-      <c r="R31" s="76"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="47"/>
+      <c r="Q31" s="62"/>
+      <c r="R31" s="63"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="40">
+      <c r="A32" s="33">
         <v>274</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="23" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="21">
         <v>45537</v>
       </c>
-      <c r="F32" s="26">
+      <c r="F32" s="21">
         <v>45902</v>
       </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="39"/>
-      <c r="P32" s="64"/>
-      <c r="Q32" s="71"/>
-      <c r="R32" s="72"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="59"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="40">
+      <c r="A33" s="33">
         <v>276</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="23" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E33" s="21">
         <v>45608</v>
       </c>
-      <c r="F33" s="26">
+      <c r="F33" s="21">
         <v>46256</v>
       </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="44" t="s">
+      <c r="G33" s="31"/>
+      <c r="H33" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="37"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="39"/>
-      <c r="P33" s="64"/>
-      <c r="Q33" s="71"/>
-      <c r="R33" s="72"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="59"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="40">
+      <c r="A34" s="33">
         <v>278</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -2135,25 +2076,25 @@
       <c r="D34" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E34" s="21">
         <v>45691</v>
       </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="45"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="55"/>
-      <c r="O34" s="45"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="88"/>
-      <c r="R34" s="89"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="51"/>
+      <c r="P34" s="43"/>
+      <c r="Q34" s="75"/>
+      <c r="R34" s="76"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="40">
+      <c r="A35" s="33">
         <v>279</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -2165,25 +2106,25 @@
       <c r="D35" s="10">
         <v>91</v>
       </c>
-      <c r="E35" s="26">
+      <c r="E35" s="21">
         <v>45722</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="45"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="88"/>
-      <c r="R35" s="89"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="75"/>
+      <c r="R35" s="76"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="40">
+      <c r="A36" s="33">
         <v>280</v>
       </c>
       <c r="B36" s="8" t="s">
@@ -2195,25 +2136,25 @@
       <c r="D36" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="21">
         <v>45769</v>
       </c>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="88"/>
-      <c r="R36" s="89"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="75"/>
+      <c r="R36" s="76"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="40">
+      <c r="A37" s="33">
         <v>281</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -2225,22 +2166,22 @@
       <c r="D37" s="10">
         <v>151.66999999999999</v>
       </c>
-      <c r="E37" s="26">
+      <c r="E37" s="21">
         <v>45748</v>
       </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="55"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="55"/>
-      <c r="Q37" s="88"/>
-      <c r="R37" s="89"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="43"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="43">

</xml_diff>